<commit_message>
Support reading .xlsb files.
</commit_message>
<xml_diff>
--- a/test/Resources/CollapsedHide.xlsx
+++ b/test/Resources/CollapsedHide.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anders\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ExcelDataReader\test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2AF6C8-E84F-445E-AA10-335FFE4AEE50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15435"/>
+    <workbookView xWindow="5130" yWindow="3900" windowWidth="20685" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
@@ -403,6 +404,8 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>

</xml_diff>